<commit_message>
TS Jatai files changes 05/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Input New Suggestion.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Input New Suggestion.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t>Passage</t>
   </si>
@@ -143,21 +143,6 @@
     <t>N[mithuS]</t>
   </si>
   <si>
-    <t>12[trapuSca]</t>
-  </si>
-  <si>
-    <t>12[mithuScarantam]</t>
-  </si>
-  <si>
-    <t>P[Scandra]</t>
-  </si>
-  <si>
-    <t>12[suScandra]</t>
-  </si>
-  <si>
-    <t>12[sa(gg)skuru</t>
-  </si>
-  <si>
     <t>N[nicAd]</t>
   </si>
   <si>
@@ -174,18 +159,6 @@
   </si>
   <si>
     <t>N[pratic]</t>
-  </si>
-  <si>
-    <t>12[samaskurvata]</t>
-  </si>
-  <si>
-    <t>12[paribBuja]</t>
-  </si>
-  <si>
-    <t>12[paricCAyA]</t>
-  </si>
-  <si>
-    <t>12[praticCinnam]</t>
   </si>
   <si>
     <t>Im</t>
@@ -215,44 +188,86 @@
     <t>N[I]</t>
   </si>
   <si>
-    <t>12 [I mandrAsu]</t>
-  </si>
-  <si>
     <t>N[t]</t>
   </si>
   <si>
     <t>N[n]</t>
   </si>
   <si>
-    <t>12 [tvai]</t>
-  </si>
-  <si>
-    <t>12[nvai]</t>
-  </si>
-  <si>
     <t>P[taBAna]</t>
   </si>
   <si>
-    <t>12[uttaBAna]</t>
+    <t>N[suS]</t>
   </si>
   <si>
-    <t>another idea to give 12 combine First Padam and next padam</t>
+    <t>iqdam</t>
   </si>
   <si>
-    <t>12[nicAduccA]</t>
+    <t>uq</t>
+  </si>
+  <si>
+    <t>naqH</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Normal Rule of uv</t>
+  </si>
+  <si>
+    <t>vaqyam</t>
+  </si>
+  <si>
+    <t>tvAq</t>
+  </si>
+  <si>
+    <t>P[u+u=U]</t>
+  </si>
+  <si>
+    <t>P[av]</t>
+  </si>
+  <si>
+    <t>Should we just give U saying it elongates</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>maqtara$m</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>N superfluous??</t>
+  </si>
+  <si>
+    <t>U+Sh</t>
+  </si>
+  <si>
+    <t>P[u+u=U] P[Sh]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -430,206 +445,207 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -914,9 +930,9 @@
   <dimension ref="A1:V1580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U11" sqref="U11"/>
+      <selection pane="bottomLeft" activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1386,7 +1402,7 @@
     <col min="16374" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="6" customFormat="1" ht="108" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12" t="s">
@@ -1443,14 +1459,12 @@
       <c r="T1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="70" t="s">
-        <v>69</v>
-      </c>
+      <c r="U1" s="70"/>
       <c r="V1" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="11"/>
@@ -1477,12 +1491,10 @@
       <c r="T2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="19" t="s">
-        <v>38</v>
-      </c>
+      <c r="U2" s="19"/>
       <c r="V2" s="29"/>
     </row>
-    <row r="3" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="11"/>
@@ -1508,7 +1520,7 @@
       <c r="U3" s="19"/>
       <c r="V3" s="29"/>
     </row>
-    <row r="4" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="11"/>
@@ -1535,12 +1547,10 @@
       <c r="T4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="U4" s="19" t="s">
-        <v>39</v>
-      </c>
+      <c r="U4" s="19"/>
       <c r="V4" s="29"/>
     </row>
-    <row r="5" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="11"/>
@@ -1566,7 +1576,7 @@
       <c r="U5" s="19"/>
       <c r="V5" s="29"/>
     </row>
-    <row r="6" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="11"/>
@@ -1587,14 +1597,16 @@
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
       <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19" t="s">
-        <v>41</v>
+      <c r="S6" s="19" t="s">
+        <v>35</v>
       </c>
+      <c r="T6" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="U6" s="19"/>
       <c r="V6" s="29"/>
     </row>
-    <row r="7" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="11"/>
@@ -1615,16 +1627,12 @@
       <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
       <c r="R7" s="19"/>
-      <c r="S7" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="T7" s="19" t="s">
-        <v>40</v>
-      </c>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
       <c r="U7" s="19"/>
       <c r="V7" s="29"/>
     </row>
-    <row r="8" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="11"/>
@@ -1649,14 +1657,12 @@
         <v>35</v>
       </c>
       <c r="T8" s="19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
-      <c r="U8" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="U8" s="19"/>
       <c r="V8" s="18"/>
     </row>
-    <row r="9" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="11"/>
@@ -1682,7 +1688,7 @@
       <c r="U9" s="19"/>
       <c r="V9" s="29"/>
     </row>
-    <row r="10" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="11"/>
@@ -1707,14 +1713,12 @@
         <v>35</v>
       </c>
       <c r="T10" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
-      <c r="U10" s="19" t="s">
-        <v>70</v>
-      </c>
+      <c r="U10" s="19"/>
       <c r="V10" s="29"/>
     </row>
-    <row r="11" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="11"/>
@@ -1740,7 +1744,7 @@
       <c r="U11" s="19"/>
       <c r="V11" s="29"/>
     </row>
-    <row r="12" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="11"/>
@@ -1763,12 +1767,10 @@
       <c r="R12" s="19"/>
       <c r="S12" s="19"/>
       <c r="T12" s="19"/>
-      <c r="U12" s="19" t="s">
-        <v>49</v>
-      </c>
+      <c r="U12" s="19"/>
       <c r="V12" s="29"/>
     </row>
-    <row r="13" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="11"/>
@@ -1792,12 +1794,12 @@
         <v>35</v>
       </c>
       <c r="T13" s="19" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="U13" s="19"/>
       <c r="V13" s="29"/>
     </row>
-    <row r="14" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="11"/>
@@ -1822,14 +1824,12 @@
         <v>35</v>
       </c>
       <c r="T14" s="19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
-      <c r="U14" s="19" t="s">
-        <v>50</v>
-      </c>
+      <c r="U14" s="19"/>
       <c r="V14" s="29"/>
     </row>
-    <row r="15" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="11"/>
@@ -1855,7 +1855,7 @@
       <c r="U15" s="19"/>
       <c r="V15" s="18"/>
     </row>
-    <row r="16" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="11"/>
@@ -1880,14 +1880,12 @@
         <v>35</v>
       </c>
       <c r="T16" s="19" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
-      <c r="U16" s="19" t="s">
-        <v>51</v>
-      </c>
+      <c r="U16" s="19"/>
       <c r="V16" s="29"/>
     </row>
-    <row r="17" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="11"/>
@@ -1913,7 +1911,7 @@
       <c r="U17" s="19"/>
       <c r="V17" s="29"/>
     </row>
-    <row r="18" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="11"/>
@@ -1938,14 +1936,12 @@
         <v>35</v>
       </c>
       <c r="T18" s="19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
-      <c r="U18" s="19" t="s">
-        <v>52</v>
-      </c>
+      <c r="U18" s="19"/>
       <c r="V18" s="29"/>
     </row>
-    <row r="19" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="11"/>
@@ -1971,7 +1967,7 @@
       <c r="U19" s="19"/>
       <c r="V19" s="29"/>
     </row>
-    <row r="20" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="11"/>
@@ -1995,7 +1991,7 @@
       <c r="U20" s="19"/>
       <c r="V20" s="18"/>
     </row>
-    <row r="21" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="11"/>
@@ -2010,24 +2006,22 @@
       <c r="L21" s="25"/>
       <c r="M21" s="7"/>
       <c r="N21" s="26" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="19"/>
       <c r="Q21" s="19"/>
       <c r="R21" s="19"/>
       <c r="S21" s="19" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="T21" s="19" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
-      <c r="U21" s="19" t="s">
-        <v>62</v>
-      </c>
+      <c r="U21" s="19"/>
       <c r="V21" s="29"/>
     </row>
-    <row r="22" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="11"/>
@@ -2042,7 +2036,7 @@
       <c r="L22" s="25"/>
       <c r="M22" s="7"/>
       <c r="N22" s="26" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="19"/>
@@ -2053,7 +2047,7 @@
       <c r="U22" s="19"/>
       <c r="V22" s="29"/>
     </row>
-    <row r="23" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="11"/>
@@ -2068,24 +2062,22 @@
       <c r="L23" s="25"/>
       <c r="M23" s="7"/>
       <c r="N23" s="71" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="19"/>
       <c r="Q23" s="19"/>
       <c r="R23" s="19"/>
       <c r="S23" s="19" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="T23" s="19" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
-      <c r="U23" s="19" t="s">
-        <v>65</v>
-      </c>
+      <c r="U23" s="19"/>
       <c r="V23" s="18"/>
     </row>
-    <row r="24" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="11"/>
@@ -2100,7 +2092,7 @@
       <c r="L24" s="25"/>
       <c r="M24" s="7"/>
       <c r="N24" s="26" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="O24" s="9"/>
       <c r="P24" s="19"/>
@@ -2111,7 +2103,7 @@
       <c r="U24" s="19"/>
       <c r="V24" s="29"/>
     </row>
-    <row r="25" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="11"/>
@@ -2126,24 +2118,22 @@
       <c r="L25" s="25"/>
       <c r="M25" s="7"/>
       <c r="N25" s="26" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="O25" s="9"/>
       <c r="P25" s="19"/>
       <c r="Q25" s="19"/>
       <c r="R25" s="19"/>
       <c r="S25" s="19" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="T25" s="19" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
-      <c r="U25" s="19" t="s">
-        <v>66</v>
-      </c>
+      <c r="U25" s="19"/>
       <c r="V25" s="29"/>
     </row>
-    <row r="26" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="11"/>
@@ -2158,7 +2148,7 @@
       <c r="L26" s="25"/>
       <c r="M26" s="7"/>
       <c r="N26" s="26" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="19"/>
@@ -2169,7 +2159,7 @@
       <c r="U26" s="19"/>
       <c r="V26" s="29"/>
     </row>
-    <row r="27" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="11"/>
@@ -2184,7 +2174,7 @@
       <c r="L27" s="25"/>
       <c r="M27" s="7"/>
       <c r="N27" s="26" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="O27" s="9"/>
       <c r="P27" s="19"/>
@@ -2192,12 +2182,10 @@
       <c r="R27" s="19"/>
       <c r="S27" s="19"/>
       <c r="T27" s="19"/>
-      <c r="U27" s="19" t="s">
-        <v>68</v>
-      </c>
+      <c r="U27" s="19"/>
       <c r="V27" s="29"/>
     </row>
-    <row r="28" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="42"/>
       <c r="E28" s="36"/>
       <c r="F28" s="36"/>
@@ -2209,22 +2197,22 @@
       <c r="L28" s="25"/>
       <c r="M28" s="7"/>
       <c r="N28" s="26" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="O28" s="8"/>
       <c r="P28" s="19"/>
       <c r="Q28" s="19"/>
       <c r="R28" s="19"/>
       <c r="S28" s="19" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="T28" s="19" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="U28" s="19"/>
       <c r="V28" s="29"/>
     </row>
-    <row r="29" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="11"/>
@@ -2248,7 +2236,7 @@
       <c r="U29" s="19"/>
       <c r="V29" s="29"/>
     </row>
-    <row r="30" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="11"/>
@@ -2262,7 +2250,9 @@
       <c r="K30" s="5"/>
       <c r="L30" s="25"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="26"/>
+      <c r="N30" s="26" t="s">
+        <v>57</v>
+      </c>
       <c r="O30" s="9"/>
       <c r="P30" s="19"/>
       <c r="Q30" s="19"/>
@@ -2272,7 +2262,7 @@
       <c r="U30" s="19"/>
       <c r="V30" s="29"/>
     </row>
-    <row r="31" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="11"/>
@@ -2286,17 +2276,23 @@
       <c r="K31" s="5"/>
       <c r="L31" s="25"/>
       <c r="M31" s="7"/>
-      <c r="N31" s="5"/>
+      <c r="N31" s="72" t="s">
+        <v>58</v>
+      </c>
       <c r="O31" s="9"/>
       <c r="P31" s="19"/>
       <c r="Q31" s="19"/>
       <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
+      <c r="S31" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
+      <c r="U31" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="V31" s="18"/>
     </row>
-    <row r="32" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="11"/>
@@ -2310,9 +2306,13 @@
       <c r="K32" s="5"/>
       <c r="L32" s="25"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="26"/>
+      <c r="N32" s="26" t="s">
+        <v>59</v>
+      </c>
       <c r="O32" s="9"/>
-      <c r="P32" s="19"/>
+      <c r="P32" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="Q32" s="19"/>
       <c r="R32" s="19"/>
       <c r="S32" s="19"/>
@@ -2320,7 +2320,7 @@
       <c r="U32" s="19"/>
       <c r="V32" s="29"/>
     </row>
-    <row r="33" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="11"/>
@@ -2334,17 +2334,25 @@
       <c r="K33" s="5"/>
       <c r="L33" s="25"/>
       <c r="M33" s="7"/>
-      <c r="N33" s="26"/>
+      <c r="N33" s="26" t="s">
+        <v>62</v>
+      </c>
       <c r="O33" s="9"/>
       <c r="P33" s="19"/>
       <c r="Q33" s="19"/>
       <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
+      <c r="S33" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="T33" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="U33" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="V33" s="29"/>
     </row>
-    <row r="34" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="11"/>
@@ -2358,17 +2366,21 @@
       <c r="K34" s="5"/>
       <c r="L34" s="25"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="26"/>
+      <c r="N34" s="26" t="s">
+        <v>58</v>
+      </c>
       <c r="O34" s="9"/>
       <c r="P34" s="19"/>
       <c r="Q34" s="19"/>
       <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
+      <c r="S34" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="T34" s="19"/>
       <c r="U34" s="19"/>
       <c r="V34" s="29"/>
     </row>
-    <row r="35" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="11"/>
@@ -2382,17 +2394,25 @@
       <c r="K35" s="5"/>
       <c r="L35" s="25"/>
       <c r="M35" s="7"/>
-      <c r="N35" s="26"/>
+      <c r="N35" s="26" t="s">
+        <v>63</v>
+      </c>
       <c r="O35" s="9"/>
-      <c r="P35" s="19"/>
+      <c r="P35" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="Q35" s="19"/>
       <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19"/>
+      <c r="S35" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="T35" s="19" t="s">
+        <v>65</v>
+      </c>
       <c r="U35" s="19"/>
       <c r="V35" s="29"/>
     </row>
-    <row r="36" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="11"/>
@@ -2406,17 +2426,25 @@
       <c r="K36" s="5"/>
       <c r="L36" s="25"/>
       <c r="M36" s="7"/>
-      <c r="N36" s="26"/>
+      <c r="N36" s="26" t="s">
+        <v>58</v>
+      </c>
       <c r="O36" s="9"/>
       <c r="P36" s="19"/>
       <c r="Q36" s="19"/>
       <c r="R36" s="19"/>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19"/>
-      <c r="U36" s="19"/>
+      <c r="S36" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="T36" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="U36" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="V36" s="29"/>
     </row>
-    <row r="37" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="11"/>
@@ -2430,17 +2458,23 @@
       <c r="K37" s="5"/>
       <c r="L37" s="25"/>
       <c r="M37" s="7"/>
-      <c r="N37" s="26"/>
+      <c r="N37" s="26" t="s">
+        <v>23</v>
+      </c>
       <c r="O37" s="9"/>
       <c r="P37" s="19"/>
       <c r="Q37" s="19"/>
       <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
+      <c r="S37" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="T37" s="19" t="s">
+        <v>73</v>
+      </c>
       <c r="U37" s="19"/>
       <c r="V37" s="29"/>
     </row>
-    <row r="38" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="11"/>
@@ -2454,9 +2488,13 @@
       <c r="K38" s="5"/>
       <c r="L38" s="25"/>
       <c r="M38" s="7"/>
-      <c r="N38" s="26"/>
+      <c r="N38" s="26" t="s">
+        <v>68</v>
+      </c>
       <c r="O38" s="9"/>
-      <c r="P38" s="19"/>
+      <c r="P38" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="Q38" s="19"/>
       <c r="R38" s="19"/>
       <c r="S38" s="19"/>
@@ -2464,7 +2502,7 @@
       <c r="U38" s="19"/>
       <c r="V38" s="29"/>
     </row>
-    <row r="39" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="11"/>
@@ -2488,7 +2526,7 @@
       <c r="U39" s="19"/>
       <c r="V39" s="18"/>
     </row>
-    <row r="40" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D40" s="42"/>
       <c r="E40" s="36"/>
       <c r="F40" s="36"/>
@@ -2508,7 +2546,7 @@
       <c r="T40" s="19"/>
       <c r="U40" s="19"/>
     </row>
-    <row r="41" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D41" s="42"/>
       <c r="E41" s="36"/>
       <c r="F41" s="36"/>
@@ -2529,7 +2567,7 @@
       <c r="U41" s="19"/>
       <c r="V41" s="29"/>
     </row>
-    <row r="42" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="11"/>
@@ -2553,7 +2591,7 @@
       <c r="U42" s="19"/>
       <c r="V42" s="29"/>
     </row>
-    <row r="43" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="11"/>
@@ -2577,7 +2615,7 @@
       <c r="U43" s="19"/>
       <c r="V43" s="29"/>
     </row>
-    <row r="44" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="11"/>
@@ -2601,7 +2639,7 @@
       <c r="U44" s="19"/>
       <c r="V44" s="29"/>
     </row>
-    <row r="45" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="11"/>
@@ -2625,7 +2663,7 @@
       <c r="U45" s="19"/>
       <c r="V45" s="29"/>
     </row>
-    <row r="46" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="11"/>
@@ -2649,7 +2687,7 @@
       <c r="U46" s="19"/>
       <c r="V46" s="29"/>
     </row>
-    <row r="47" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="11"/>
@@ -2673,7 +2711,7 @@
       <c r="U47" s="19"/>
       <c r="V47" s="29"/>
     </row>
-    <row r="48" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="11"/>
@@ -2697,7 +2735,7 @@
       <c r="U48" s="19"/>
       <c r="V48" s="18"/>
     </row>
-    <row r="49" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="11"/>
@@ -2721,7 +2759,7 @@
       <c r="U49" s="19"/>
       <c r="V49" s="29"/>
     </row>
-    <row r="50" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D50" s="42"/>
       <c r="E50" s="36"/>
       <c r="F50" s="36"/>
@@ -2742,7 +2780,7 @@
       <c r="U50" s="19"/>
       <c r="V50" s="18"/>
     </row>
-    <row r="51" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D51" s="42"/>
       <c r="E51" s="36"/>
       <c r="F51" s="36"/>
@@ -2763,7 +2801,7 @@
       <c r="U51" s="19"/>
       <c r="V51" s="29"/>
     </row>
-    <row r="52" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="11"/>
@@ -2787,7 +2825,7 @@
       <c r="U52" s="19"/>
       <c r="V52" s="29"/>
     </row>
-    <row r="53" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D53" s="42"/>
       <c r="E53" s="36"/>
       <c r="F53" s="36"/>
@@ -2808,7 +2846,7 @@
       <c r="U53" s="19"/>
       <c r="V53" s="29"/>
     </row>
-    <row r="54" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="11"/>
@@ -2832,7 +2870,7 @@
       <c r="U54" s="19"/>
       <c r="V54" s="29"/>
     </row>
-    <row r="55" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="11"/>
@@ -2856,7 +2894,7 @@
       <c r="U55" s="19"/>
       <c r="V55" s="29"/>
     </row>
-    <row r="56" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="11"/>
@@ -2880,7 +2918,7 @@
       <c r="U56" s="19"/>
       <c r="V56" s="29"/>
     </row>
-    <row r="57" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="11"/>
@@ -2904,7 +2942,7 @@
       <c r="U57" s="19"/>
       <c r="V57" s="29"/>
     </row>
-    <row r="58" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="11"/>
@@ -2928,7 +2966,7 @@
       <c r="U58" s="19"/>
       <c r="V58" s="29"/>
     </row>
-    <row r="59" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="11"/>
@@ -2952,7 +2990,7 @@
       <c r="U59" s="19"/>
       <c r="V59" s="29"/>
     </row>
-    <row r="60" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="11"/>
@@ -2976,7 +3014,7 @@
       <c r="U60" s="19"/>
       <c r="V60" s="18"/>
     </row>
-    <row r="61" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D61" s="42"/>
       <c r="E61" s="36"/>
       <c r="F61" s="36"/>
@@ -2997,7 +3035,7 @@
       <c r="U61" s="19"/>
       <c r="V61" s="18"/>
     </row>
-    <row r="62" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D62" s="42"/>
       <c r="E62" s="36"/>
       <c r="F62" s="36"/>
@@ -3018,7 +3056,7 @@
       <c r="U62" s="19"/>
       <c r="V62" s="29"/>
     </row>
-    <row r="63" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D63" s="42"/>
       <c r="E63" s="36"/>
       <c r="F63" s="36"/>
@@ -3039,7 +3077,7 @@
       <c r="U63" s="19"/>
       <c r="V63" s="29"/>
     </row>
-    <row r="64" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="11"/>
@@ -3063,7 +3101,7 @@
       <c r="U64" s="19"/>
       <c r="V64" s="29"/>
     </row>
-    <row r="65" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="11"/>
@@ -3087,7 +3125,7 @@
       <c r="U65" s="19"/>
       <c r="V65" s="29"/>
     </row>
-    <row r="66" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="11"/>
@@ -3111,7 +3149,7 @@
       <c r="U66" s="19"/>
       <c r="V66" s="29"/>
     </row>
-    <row r="67" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="11"/>
@@ -3135,7 +3173,7 @@
       <c r="U67" s="19"/>
       <c r="V67" s="29"/>
     </row>
-    <row r="68" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="11"/>
@@ -3159,7 +3197,7 @@
       <c r="U68" s="19"/>
       <c r="V68" s="29"/>
     </row>
-    <row r="69" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="11"/>
@@ -3183,7 +3221,7 @@
       <c r="U69" s="19"/>
       <c r="V69" s="29"/>
     </row>
-    <row r="70" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="11"/>
@@ -3207,7 +3245,7 @@
       <c r="U70" s="19"/>
       <c r="V70" s="29"/>
     </row>
-    <row r="71" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D71" s="42"/>
       <c r="E71" s="36"/>
       <c r="F71" s="36"/>
@@ -3228,7 +3266,7 @@
       <c r="U71" s="19"/>
       <c r="V71" s="18"/>
     </row>
-    <row r="72" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D72" s="42"/>
       <c r="E72" s="36"/>
       <c r="F72" s="36"/>
@@ -3249,7 +3287,7 @@
       <c r="U72" s="19"/>
       <c r="V72" s="29"/>
     </row>
-    <row r="73" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="11"/>
@@ -3273,7 +3311,7 @@
       <c r="U73" s="19"/>
       <c r="V73" s="18"/>
     </row>
-    <row r="74" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D74" s="42"/>
       <c r="E74" s="36"/>
       <c r="F74" s="36"/>
@@ -3294,7 +3332,7 @@
       <c r="U74" s="19"/>
       <c r="V74" s="29"/>
     </row>
-    <row r="75" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D75" s="42"/>
       <c r="E75" s="36"/>
       <c r="F75" s="36"/>
@@ -3315,7 +3353,7 @@
       <c r="U75" s="19"/>
       <c r="V75" s="18"/>
     </row>
-    <row r="76" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="11"/>
@@ -3339,7 +3377,7 @@
       <c r="U76" s="19"/>
       <c r="V76" s="29"/>
     </row>
-    <row r="77" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D77" s="42"/>
       <c r="E77" s="36"/>
       <c r="F77" s="36"/>
@@ -3360,7 +3398,7 @@
       <c r="U77" s="19"/>
       <c r="V77" s="18"/>
     </row>
-    <row r="78" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D78" s="42"/>
       <c r="E78" s="36"/>
       <c r="F78" s="36"/>
@@ -3381,7 +3419,7 @@
       <c r="U78" s="19"/>
       <c r="V78" s="29"/>
     </row>
-    <row r="79" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="11"/>
@@ -3405,7 +3443,7 @@
       <c r="U79" s="19"/>
       <c r="V79" s="29"/>
     </row>
-    <row r="80" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D80" s="42"/>
       <c r="E80" s="36"/>
       <c r="F80" s="36"/>
@@ -3426,7 +3464,7 @@
       <c r="U80" s="19"/>
       <c r="V80" s="29"/>
     </row>
-    <row r="81" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D81" s="42"/>
       <c r="E81" s="36"/>
       <c r="F81" s="36"/>
@@ -3447,7 +3485,7 @@
       <c r="U81" s="19"/>
       <c r="V81" s="29"/>
     </row>
-    <row r="82" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D82" s="42"/>
       <c r="E82" s="36"/>
       <c r="F82" s="36"/>
@@ -3468,7 +3506,7 @@
       <c r="U82" s="19"/>
       <c r="V82" s="29"/>
     </row>
-    <row r="83" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D83" s="42"/>
       <c r="E83" s="36"/>
       <c r="F83" s="36"/>
@@ -3489,7 +3527,7 @@
       <c r="U83" s="19"/>
       <c r="V83" s="29"/>
     </row>
-    <row r="84" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D84" s="42"/>
       <c r="E84" s="36"/>
       <c r="F84" s="36"/>
@@ -3510,7 +3548,7 @@
       <c r="U84" s="19"/>
       <c r="V84" s="29"/>
     </row>
-    <row r="85" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D85" s="42"/>
       <c r="E85" s="36"/>
       <c r="F85" s="36"/>
@@ -3531,7 +3569,7 @@
       <c r="U85" s="19"/>
       <c r="V85" s="29"/>
     </row>
-    <row r="86" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D86" s="42"/>
       <c r="E86" s="36"/>
       <c r="F86" s="36"/>
@@ -3552,7 +3590,7 @@
       <c r="U86" s="19"/>
       <c r="V86" s="18"/>
     </row>
-    <row r="87" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D87" s="42"/>
       <c r="E87" s="36"/>
       <c r="F87" s="36"/>
@@ -3573,7 +3611,7 @@
       <c r="U87" s="19"/>
       <c r="V87" s="29"/>
     </row>
-    <row r="88" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D88" s="42"/>
       <c r="E88" s="36"/>
       <c r="F88" s="36"/>
@@ -3594,7 +3632,7 @@
       <c r="U88" s="19"/>
       <c r="V88" s="29"/>
     </row>
-    <row r="89" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D89" s="42"/>
       <c r="E89" s="36"/>
       <c r="F89" s="36"/>
@@ -3615,7 +3653,7 @@
       <c r="U89" s="19"/>
       <c r="V89" s="29"/>
     </row>
-    <row r="90" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D90" s="42"/>
       <c r="E90" s="36"/>
       <c r="F90" s="36"/>
@@ -3636,7 +3674,7 @@
       <c r="U90" s="19"/>
       <c r="V90" s="18"/>
     </row>
-    <row r="91" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="11"/>
@@ -3660,7 +3698,7 @@
       <c r="U91" s="19"/>
       <c r="V91" s="18"/>
     </row>
-    <row r="92" spans="1:22" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="11"/>
@@ -3684,7 +3722,7 @@
       <c r="U92" s="19"/>
       <c r="V92" s="29"/>
     </row>
-    <row r="93" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D93" s="42"/>
       <c r="E93" s="36"/>
       <c r="F93" s="36"/>
@@ -3704,7 +3742,7 @@
       <c r="T93" s="9"/>
       <c r="U93" s="9"/>
     </row>
-    <row r="94" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D94" s="42"/>
       <c r="E94" s="36"/>
       <c r="F94" s="36"/>
@@ -3725,7 +3763,7 @@
       <c r="U94" s="21"/>
       <c r="V94" s="18"/>
     </row>
-    <row r="95" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D95" s="42"/>
       <c r="E95" s="36"/>
       <c r="F95" s="36"/>
@@ -3745,7 +3783,7 @@
       <c r="T95" s="9"/>
       <c r="U95" s="9"/>
     </row>
-    <row r="96" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D96" s="42"/>
       <c r="E96" s="36"/>
       <c r="F96" s="36"/>
@@ -3765,7 +3803,7 @@
       <c r="T96" s="9"/>
       <c r="U96" s="9"/>
     </row>
-    <row r="97" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D97" s="42"/>
       <c r="E97" s="36"/>
       <c r="F97" s="36"/>
@@ -3785,7 +3823,7 @@
       <c r="T97" s="9"/>
       <c r="U97" s="9"/>
     </row>
-    <row r="98" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D98" s="42"/>
       <c r="E98" s="36"/>
       <c r="F98" s="36"/>
@@ -3806,7 +3844,7 @@
       <c r="U98" s="9"/>
       <c r="V98" s="29"/>
     </row>
-    <row r="99" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D99" s="42"/>
       <c r="E99" s="36"/>
       <c r="F99" s="36"/>
@@ -3827,7 +3865,7 @@
       <c r="U99" s="9"/>
       <c r="V99" s="18"/>
     </row>
-    <row r="100" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D100" s="42"/>
       <c r="E100" s="36"/>
       <c r="F100" s="36"/>
@@ -3847,7 +3885,7 @@
       <c r="T100" s="9"/>
       <c r="U100" s="9"/>
     </row>
-    <row r="101" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D101" s="42"/>
       <c r="E101" s="36"/>
       <c r="F101" s="36"/>
@@ -3868,7 +3906,7 @@
       <c r="U101" s="9"/>
       <c r="V101" s="18"/>
     </row>
-    <row r="102" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D102" s="42"/>
       <c r="E102" s="36"/>
       <c r="F102" s="36"/>
@@ -3888,7 +3926,7 @@
       <c r="T102" s="9"/>
       <c r="U102" s="9"/>
     </row>
-    <row r="103" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D103" s="42"/>
       <c r="E103" s="36"/>
       <c r="F103" s="36"/>
@@ -3908,7 +3946,7 @@
       <c r="T103" s="9"/>
       <c r="U103" s="9"/>
     </row>
-    <row r="104" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D104" s="42"/>
       <c r="E104" s="36"/>
       <c r="F104" s="36"/>
@@ -3928,7 +3966,7 @@
       <c r="T104" s="9"/>
       <c r="U104" s="9"/>
     </row>
-    <row r="105" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D105" s="42"/>
       <c r="E105" s="36"/>
       <c r="F105" s="36"/>
@@ -3949,7 +3987,7 @@
       <c r="U105" s="9"/>
       <c r="V105" s="29"/>
     </row>
-    <row r="106" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D106" s="42"/>
       <c r="E106" s="36"/>
       <c r="F106" s="36"/>
@@ -3969,7 +4007,7 @@
       <c r="T106" s="9"/>
       <c r="U106" s="9"/>
     </row>
-    <row r="107" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D107" s="42"/>
       <c r="E107" s="36"/>
       <c r="F107" s="36"/>
@@ -3989,7 +4027,7 @@
       <c r="T107" s="9"/>
       <c r="U107" s="9"/>
     </row>
-    <row r="108" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D108" s="42"/>
       <c r="E108" s="36"/>
       <c r="F108" s="36"/>
@@ -4009,7 +4047,7 @@
       <c r="T108" s="9"/>
       <c r="U108" s="9"/>
     </row>
-    <row r="109" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D109" s="42"/>
       <c r="E109" s="36"/>
       <c r="F109" s="36"/>
@@ -4030,7 +4068,7 @@
       <c r="U109" s="9"/>
       <c r="V109" s="20"/>
     </row>
-    <row r="110" spans="4:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:22" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D110" s="42"/>
       <c r="E110" s="36"/>
       <c r="F110" s="36"/>

</xml_diff>